<commit_message>
Added tabs to aroms modal
</commit_message>
<xml_diff>
--- a/info/список ароматизаторов.xlsx
+++ b/info/список ароматизаторов.xlsx
@@ -2,15 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Capella" sheetId="3" r:id="rId3"/>
+    <sheet name="FlavourArt" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="542">
   <si>
     <t>A</t>
   </si>
@@ -6150,12 +6152,396 @@
   </si>
   <si>
     <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>Apple Pie V2 (Яблочный пирог 2)</t>
+  </si>
+  <si>
+    <t>Banana (Банан)</t>
+  </si>
+  <si>
+    <t>Bavarian Cream (Баварский крем)</t>
+  </si>
+  <si>
+    <t>Blackberry (Ежевика)</t>
+  </si>
+  <si>
+    <t>Bubble Gum (Жвачка)</t>
+  </si>
+  <si>
+    <t>Butter Cream (Крем)</t>
+  </si>
+  <si>
+    <t>Cake Batter (Тесто для кекса)</t>
+  </si>
+  <si>
+    <t>Cantaloupe (Мускусная дыня)</t>
+  </si>
+  <si>
+    <t>Cappuccino (Каппучино)</t>
+  </si>
+  <si>
+    <t>Caramel V2 (Карамель 2)</t>
+  </si>
+  <si>
+    <t>Cereal 27 (Кукурузные хлопья)</t>
+  </si>
+  <si>
+    <t>Cherry (Wild) w/Stevia (Дикая вишня и стевия)</t>
+  </si>
+  <si>
+    <t>Chocolate Coconut Almond (Шоколад кокос миндаль)</t>
+  </si>
+  <si>
+    <t>Chocolate Glazed Doughnut (Глазированный шаколадный пончик)</t>
+  </si>
+  <si>
+    <t>Chocolate Raspberry (Малина с шоколадом)</t>
+  </si>
+  <si>
+    <t>Cola (Кола)</t>
+  </si>
+  <si>
+    <t>Concord Grape w/Stevia (Конкорд и стевия)</t>
+  </si>
+  <si>
+    <t>Cool Mint (Мятная свежесть)</t>
+  </si>
+  <si>
+    <t>Cranberry (Клюква)</t>
+  </si>
+  <si>
+    <t>Creamy Yogurt (Кремовый йогурт)</t>
+  </si>
+  <si>
+    <t>Double Apple (Двойное яблоко)</t>
+  </si>
+  <si>
+    <t>Double Watermelon (Двойной арбуз)</t>
+  </si>
+  <si>
+    <t>Dragon Fruit (Драгонфрут)</t>
+  </si>
+  <si>
+    <t>Funnel Cake (Торт "Муравейник")</t>
+  </si>
+  <si>
+    <t>Golden Pineapple (Золотой ананас)</t>
+  </si>
+  <si>
+    <t>Graham Cracker V2 (Грэхем крекер 2)</t>
+  </si>
+  <si>
+    <t>Grapefruit (Грейпфрут)</t>
+  </si>
+  <si>
+    <t>Greek Yogurt (Греческий йогурт)</t>
+  </si>
+  <si>
+    <t>Green Apple (Зеленое яблоко)</t>
+  </si>
+  <si>
+    <t>Grenadine (Гренадин)</t>
+  </si>
+  <si>
+    <t>Harvest Berry (Лесные ягоды)</t>
+  </si>
+  <si>
+    <t>Hazelnut (Лесной орех)</t>
+  </si>
+  <si>
+    <t>Honeydew Melon (Медовая дыня)</t>
+  </si>
+  <si>
+    <t>Jelly Candys (Конфеты желе)</t>
+  </si>
+  <si>
+    <t>Juicy Lemon (Сок лимона)</t>
+  </si>
+  <si>
+    <t>Juicy Orange (Сочный апельсин)</t>
+  </si>
+  <si>
+    <t>Juicy Peach (Сочный персик)</t>
+  </si>
+  <si>
+    <t>Kiwi (Киви)</t>
+  </si>
+  <si>
+    <t>Kiwi Strawberry (Киви и клубника)</t>
+  </si>
+  <si>
+    <t>Lemon Lime (Лимон-лайм)</t>
+  </si>
+  <si>
+    <t>Maple (Pancake Syrup) (Кленовый сироп)</t>
+  </si>
+  <si>
+    <t>Milk Chocolate Toffee (Шоколаный тоффи)</t>
+  </si>
+  <si>
+    <t>New York Cheesecake v2 (New York чизкейк v2)</t>
+  </si>
+  <si>
+    <t>Orange Creamsicle (Апельсиновое мороженное)</t>
+  </si>
+  <si>
+    <t>Orange Mango (Апельсин и манго)</t>
+  </si>
+  <si>
+    <t>Passion Fruit (Маракуйя)</t>
+  </si>
+  <si>
+    <t>Peach w/Stevia (Персик и стевия)</t>
+  </si>
+  <si>
+    <t>Peaches and Cream (Персики в крему)</t>
+  </si>
+  <si>
+    <t>Peaches and Cream v2 (Персики в крему v2)</t>
+  </si>
+  <si>
+    <t>Peanut Butter V2 (Арахисовое масло (версия 2))</t>
+  </si>
+  <si>
+    <t>Pear Flavor (Груша)</t>
+  </si>
+  <si>
+    <t>Pink Lemonades (Лимонад)</t>
+  </si>
+  <si>
+    <t>Pomegranate V2 (Гранат 2)</t>
+  </si>
+  <si>
+    <t>Raspberry (Малина)</t>
+  </si>
+  <si>
+    <t>Raspberry V2 (Малина 2)</t>
+  </si>
+  <si>
+    <t>Strawberries and Cream ( Клубника в сливках)</t>
+  </si>
+  <si>
+    <t>Strawberry Taffys (Клубничный тэфи)</t>
+  </si>
+  <si>
+    <t>Sugar Cookie v2 (Сахарное печенье v2)</t>
+  </si>
+  <si>
+    <t>Super Sweet Sucralose Sweetener (Подсластитель)</t>
+  </si>
+  <si>
+    <t>Sweet Cream (Сладкий крем)</t>
+  </si>
+  <si>
+    <t>Sweet Lychee (Сладкий личи)</t>
+  </si>
+  <si>
+    <t>Sweet Mango (Сладкий манго)</t>
+  </si>
+  <si>
+    <t>Sweet Tangerine (Сладкий мандарин)</t>
+  </si>
+  <si>
+    <t>Sweet Tangerine Rf (Сладкий мандарин)</t>
+  </si>
+  <si>
+    <t>Sweet Tea (Сладкий чай)</t>
+  </si>
+  <si>
+    <t>Sweet Watermelon (Сладкий арбуз)</t>
+  </si>
+  <si>
+    <t>Vanilla Bean Ice Cream (Ванильное мороженное)</t>
+  </si>
+  <si>
+    <t>Vanilla Cupcake V2 (Ванильный пирог)</t>
+  </si>
+  <si>
+    <t>Vanilla Custard (Ванильный кастард)</t>
+  </si>
+  <si>
+    <t>Vanilla Whipped Cream (Ванильные взбитые сливки)</t>
+  </si>
+  <si>
+    <t>Waffle (Вафли)</t>
+  </si>
+  <si>
+    <t>Yellow Peach (Желтый персик)</t>
+  </si>
+  <si>
+    <t>Apple Pie (Яблочный пирог)</t>
+  </si>
+  <si>
+    <t>Apricot (Абрикос)</t>
+  </si>
+  <si>
+    <t>Banana Split (Банановый сплит)</t>
+  </si>
+  <si>
+    <t>Blueberry (Черника)</t>
+  </si>
+  <si>
+    <t>Blueberry Cinnamon Crumble (Черничный пирог с корицей)</t>
+  </si>
+  <si>
+    <t>Blueberry Jam (Черничное варенье)</t>
+  </si>
+  <si>
+    <t>Blueberry Pomegranate (Черника и гранат)</t>
+  </si>
+  <si>
+    <t>Boston Cream Pie V2 (Бостонский кремовый пирог)</t>
+  </si>
+  <si>
+    <t>Churro (Чуррос)</t>
+  </si>
+  <si>
+    <t>Cinnamon Danish Swirl V2 (Датский завиток с корицей 2)</t>
+  </si>
+  <si>
+    <t>Coconut (Кокос)</t>
+  </si>
+  <si>
+    <t>French Vanilla (Французкая ваниль)</t>
+  </si>
+  <si>
+    <t>Glazed Doughnut (Глазированный пончик)</t>
+  </si>
+  <si>
+    <t>Italian Lemon Sicily (Сицилийский лимон)</t>
+  </si>
+  <si>
+    <t>Jelly Candy (Конфеты из желе)</t>
+  </si>
+  <si>
+    <t>Lemon Meringue Pie (Лимонный пирог с безе)</t>
+  </si>
+  <si>
+    <t>New York Cheesecake (New York чизкейк)</t>
+  </si>
+  <si>
+    <t>Simply Vanilla (Ваниль)</t>
+  </si>
+  <si>
+    <t>Sweet Strawberry (Сладкая клубника)</t>
+  </si>
+  <si>
+    <t>Sweet Strawberry RF (Сладкая клубника РФ)</t>
+  </si>
+  <si>
+    <t>Vanilla Custard V2 (Ванильный крем v2)</t>
+  </si>
+  <si>
+    <t>Wild Cherry (Дикая вишня)</t>
+  </si>
+  <si>
+    <t>Apple Pie (Яблочный Пирог)</t>
+  </si>
+  <si>
+    <t>Bilberry (Черника)</t>
+  </si>
+  <si>
+    <t>Biscotto Cookie (Овсяное Печенье)</t>
+  </si>
+  <si>
+    <t>Blackcurrant (Черная Смородина)</t>
+  </si>
+  <si>
+    <t>Caramel (Карамель)</t>
+  </si>
+  <si>
+    <t>Champagne (Шампанское)</t>
+  </si>
+  <si>
+    <t>Cherry (Вишня)</t>
+  </si>
+  <si>
+    <t>Citrus Mix (Цитрусовый Микс)</t>
+  </si>
+  <si>
+    <t>Classic Vanilla (Ваниль)</t>
+  </si>
+  <si>
+    <t>Custard Cream (Заварной Крем)</t>
+  </si>
+  <si>
+    <t>Forest Fruit Mix (Фруктовый Микс)</t>
+  </si>
+  <si>
+    <t>Fuji Apple (Яблоко Fuji)</t>
+  </si>
+  <si>
+    <t>Green Tea (Зеленый Чай)</t>
+  </si>
+  <si>
+    <t>Hazelnut (Лесной Орех)</t>
+  </si>
+  <si>
+    <t>Lemon Sicily (Лимон Сицилийский)</t>
+  </si>
+  <si>
+    <t>Lime Tahity Distilled (Лайм)</t>
+  </si>
+  <si>
+    <t>Mandarin (Мандарин)</t>
+  </si>
+  <si>
+    <t>Mango (Манго)</t>
+  </si>
+  <si>
+    <t>Marshmallow (Зефир)</t>
+  </si>
+  <si>
+    <t>Maxx Blend (Табак Maxx Blend)</t>
+  </si>
+  <si>
+    <t>Melon Cantaloupe (Мускусная Дыня)</t>
+  </si>
+  <si>
+    <t>Menthol (Ментол)</t>
+  </si>
+  <si>
+    <t>Meringue (Безе)</t>
+  </si>
+  <si>
+    <t>Nonna’s Cake (Пирог Нонны)</t>
+  </si>
+  <si>
+    <t>Orange (Апельсин)</t>
+  </si>
+  <si>
+    <t>Passionfruit (Маракуйя)</t>
+  </si>
+  <si>
+    <t>Soho (Табак Soho)</t>
+  </si>
+  <si>
+    <t>Spearmint (Мятная Жвачка)</t>
+  </si>
+  <si>
+    <t>Stark Apple (Яблоко Красное)</t>
+  </si>
+  <si>
+    <t>Strawberry (Клубника)</t>
+  </si>
+  <si>
+    <t>Virginia (Табак Virginia)</t>
+  </si>
+  <si>
+    <t>Watermelon (Арбуз)</t>
+  </si>
+  <si>
+    <t>White Peach (Белый Персик)</t>
+  </si>
+  <si>
+    <t>Yogurt (Йогурт)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -6515,7 +6901,7 @@
   <dimension ref="A1:B220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8305,8 +8691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11685,4 +12071,2338 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L94"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B1" t="str">
+        <f>CONCATENATE("'",A1,"'")</f>
+        <v>'Apple Pie (Яблочный пирог)'</v>
+      </c>
+      <c r="F1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1" t="s">
+        <v>411</v>
+      </c>
+      <c r="J1" t="s">
+        <v>412</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE($F$1,$H$1,B1,$J$1)</f>
+        <v>{name: 'Apple Pie (Яблочный пирог)' },</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE($F$1,$G$1,B1,$H$2,$H$1,B1,$J$1)</f>
+        <v>{id: 'Apple Pie (Яблочный пирог)', name: 'Apple Pie (Яблочный пирог)' },</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE("'",A2,"'")</f>
+        <v>'Apple Pie V2 (Яблочный пирог 2)'</v>
+      </c>
+      <c r="H2" t="s">
+        <v>413</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2" si="0">CONCATENATE($F$1,$H$1,B2,$J$1)</f>
+        <v>{name: 'Apple Pie V2 (Яблочный пирог 2)' },</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2" si="1">CONCATENATE($F$1,$G$1,B2,$H$2,$H$1,B2,$J$1)</f>
+        <v>{id: 'Apple Pie V2 (Яблочный пирог 2)', name: 'Apple Pie V2 (Яблочный пирог 2)' },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B66" si="2">CONCATENATE("'",A3,"'")</f>
+        <v>'Apricot (Абрикос)'</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="3">CONCATENATE($F$1,$H$1,B3,$J$1)</f>
+        <v>{name: 'Apricot (Абрикос)' },</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L66" si="4">CONCATENATE($F$1,$G$1,B3,$H$2,$H$1,B3,$J$1)</f>
+        <v>{id: 'Apricot (Абрикос)', name: 'Apricot (Абрикос)' },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="2"/>
+        <v>'Banana (Банан)'</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Banana (Банан)' },</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Banana (Банан)', name: 'Banana (Банан)' },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="2"/>
+        <v>'Banana Split (Банановый сплит)'</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Banana Split (Банановый сплит)' },</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Banana Split (Банановый сплит)', name: 'Banana Split (Банановый сплит)' },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>416</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="2"/>
+        <v>'Bavarian Cream (Баварский крем)'</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Bavarian Cream (Баварский крем)' },</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Bavarian Cream (Баварский крем)', name: 'Bavarian Cream (Баварский крем)' },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="2"/>
+        <v>'Blackberry (Ежевика)'</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Blackberry (Ежевика)' },</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Blackberry (Ежевика)', name: 'Blackberry (Ежевика)' },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>489</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="2"/>
+        <v>'Blueberry (Черника)'</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Blueberry (Черника)' },</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Blueberry (Черника)', name: 'Blueberry (Черника)' },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>490</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="2"/>
+        <v>'Blueberry Cinnamon Crumble (Черничный пирог с корицей)'</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Blueberry Cinnamon Crumble (Черничный пирог с корицей)' },</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Blueberry Cinnamon Crumble (Черничный пирог с корицей)', name: 'Blueberry Cinnamon Crumble (Черничный пирог с корицей)' },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>491</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="2"/>
+        <v>'Blueberry Jam (Черничное варенье)'</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Blueberry Jam (Черничное варенье)' },</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Blueberry Jam (Черничное варенье)', name: 'Blueberry Jam (Черничное варенье)' },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>492</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="2"/>
+        <v>'Blueberry Pomegranate (Черника и гранат)'</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Blueberry Pomegranate (Черника и гранат)' },</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Blueberry Pomegranate (Черника и гранат)', name: 'Blueberry Pomegranate (Черника и гранат)' },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>493</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="2"/>
+        <v>'Boston Cream Pie V2 (Бостонский кремовый пирог)'</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Boston Cream Pie V2 (Бостонский кремовый пирог)' },</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Boston Cream Pie V2 (Бостонский кремовый пирог)', name: 'Boston Cream Pie V2 (Бостонский кремовый пирог)' },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>418</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="2"/>
+        <v>'Bubble Gum (Жвачка)'</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Bubble Gum (Жвачка)' },</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Bubble Gum (Жвачка)', name: 'Bubble Gum (Жвачка)' },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="2"/>
+        <v>'Butter Cream (Крем)'</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Butter Cream (Крем)' },</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Butter Cream (Крем)', name: 'Butter Cream (Крем)' },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>420</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cake Batter (Тесто для кекса)'</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cake Batter (Тесто для кекса)' },</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cake Batter (Тесто для кекса)', name: 'Cake Batter (Тесто для кекса)' },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>421</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cantaloupe (Мускусная дыня)'</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cantaloupe (Мускусная дыня)' },</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cantaloupe (Мускусная дыня)', name: 'Cantaloupe (Мускусная дыня)' },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>422</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cappuccino (Каппучино)'</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cappuccino (Каппучино)' },</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cappuccino (Каппучино)', name: 'Cappuccino (Каппучино)' },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>423</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="2"/>
+        <v>'Caramel V2 (Карамель 2)'</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Caramel V2 (Карамель 2)' },</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Caramel V2 (Карамель 2)', name: 'Caramel V2 (Карамель 2)' },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>424</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cereal 27 (Кукурузные хлопья)'</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cereal 27 (Кукурузные хлопья)' },</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cereal 27 (Кукурузные хлопья)', name: 'Cereal 27 (Кукурузные хлопья)' },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>425</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cherry (Wild) w/Stevia (Дикая вишня и стевия)'</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cherry (Wild) w/Stevia (Дикая вишня и стевия)' },</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cherry (Wild) w/Stevia (Дикая вишня и стевия)', name: 'Cherry (Wild) w/Stevia (Дикая вишня и стевия)' },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>426</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="2"/>
+        <v>'Chocolate Coconut Almond (Шоколад кокос миндаль)'</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Chocolate Coconut Almond (Шоколад кокос миндаль)' },</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Chocolate Coconut Almond (Шоколад кокос миндаль)', name: 'Chocolate Coconut Almond (Шоколад кокос миндаль)' },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>427</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="2"/>
+        <v>'Chocolate Glazed Doughnut (Глазированный шаколадный пончик)'</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Chocolate Glazed Doughnut (Глазированный шаколадный пончик)' },</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Chocolate Glazed Doughnut (Глазированный шаколадный пончик)', name: 'Chocolate Glazed Doughnut (Глазированный шаколадный пончик)' },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>428</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="2"/>
+        <v>'Chocolate Raspberry (Малина с шоколадом)'</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Chocolate Raspberry (Малина с шоколадом)' },</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Chocolate Raspberry (Малина с шоколадом)', name: 'Chocolate Raspberry (Малина с шоколадом)' },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>494</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="2"/>
+        <v>'Churro (Чуррос)'</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Churro (Чуррос)' },</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Churro (Чуррос)', name: 'Churro (Чуррос)' },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>495</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cinnamon Danish Swirl V2 (Датский завиток с корицей 2)'</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cinnamon Danish Swirl V2 (Датский завиток с корицей 2)' },</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cinnamon Danish Swirl V2 (Датский завиток с корицей 2)', name: 'Cinnamon Danish Swirl V2 (Датский завиток с корицей 2)' },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>496</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="2"/>
+        <v>'Coconut (Кокос)'</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Coconut (Кокос)' },</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Coconut (Кокос)', name: 'Coconut (Кокос)' },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>429</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cola (Кола)'</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cola (Кола)' },</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cola (Кола)', name: 'Cola (Кола)' },</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>430</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="2"/>
+        <v>'Concord Grape w/Stevia (Конкорд и стевия)'</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Concord Grape w/Stevia (Конкорд и стевия)' },</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Concord Grape w/Stevia (Конкорд и стевия)', name: 'Concord Grape w/Stevia (Конкорд и стевия)' },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>431</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cool Mint (Мятная свежесть)'</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cool Mint (Мятная свежесть)' },</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cool Mint (Мятная свежесть)', name: 'Cool Mint (Мятная свежесть)' },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>432</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="2"/>
+        <v>'Cranberry (Клюква)'</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Cranberry (Клюква)' },</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Cranberry (Клюква)', name: 'Cranberry (Клюква)' },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>433</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="2"/>
+        <v>'Creamy Yogurt (Кремовый йогурт)'</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Creamy Yogurt (Кремовый йогурт)' },</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Creamy Yogurt (Кремовый йогурт)', name: 'Creamy Yogurt (Кремовый йогурт)' },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>434</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="2"/>
+        <v>'Double Apple (Двойное яблоко)'</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Double Apple (Двойное яблоко)' },</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Double Apple (Двойное яблоко)', name: 'Double Apple (Двойное яблоко)' },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>435</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="2"/>
+        <v>'Double Watermelon (Двойной арбуз)'</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Double Watermelon (Двойной арбуз)' },</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Double Watermelon (Двойной арбуз)', name: 'Double Watermelon (Двойной арбуз)' },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>436</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="2"/>
+        <v>'Dragon Fruit (Драгонфрут)'</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Dragon Fruit (Драгонфрут)' },</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Dragon Fruit (Драгонфрут)', name: 'Dragon Fruit (Драгонфрут)' },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" t="s">
+        <v>497</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="2"/>
+        <v>'French Vanilla (Французкая ваниль)'</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'French Vanilla (Французкая ваниль)' },</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'French Vanilla (Французкая ваниль)', name: 'French Vanilla (Французкая ваниль)' },</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" t="s">
+        <v>437</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="2"/>
+        <v>'Funnel Cake (Торт "Муравейник")'</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Funnel Cake (Торт "Муравейник")' },</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Funnel Cake (Торт "Муравейник")', name: 'Funnel Cake (Торт "Муравейник")' },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" t="s">
+        <v>498</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="2"/>
+        <v>'Glazed Doughnut (Глазированный пончик)'</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Glazed Doughnut (Глазированный пончик)' },</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Glazed Doughnut (Глазированный пончик)', name: 'Glazed Doughnut (Глазированный пончик)' },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>438</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="2"/>
+        <v>'Golden Pineapple (Золотой ананас)'</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Golden Pineapple (Золотой ананас)' },</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Golden Pineapple (Золотой ананас)', name: 'Golden Pineapple (Золотой ананас)' },</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" t="s">
+        <v>439</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="2"/>
+        <v>'Graham Cracker V2 (Грэхем крекер 2)'</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Graham Cracker V2 (Грэхем крекер 2)' },</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Graham Cracker V2 (Грэхем крекер 2)', name: 'Graham Cracker V2 (Грэхем крекер 2)' },</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" t="s">
+        <v>440</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="2"/>
+        <v>'Grapefruit (Грейпфрут)'</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Grapefruit (Грейпфрут)' },</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Grapefruit (Грейпфрут)', name: 'Grapefruit (Грейпфрут)' },</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>441</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="2"/>
+        <v>'Greek Yogurt (Греческий йогурт)'</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Greek Yogurt (Греческий йогурт)' },</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Greek Yogurt (Греческий йогурт)', name: 'Greek Yogurt (Греческий йогурт)' },</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>442</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="2"/>
+        <v>'Green Apple (Зеленое яблоко)'</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Green Apple (Зеленое яблоко)' },</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Green Apple (Зеленое яблоко)', name: 'Green Apple (Зеленое яблоко)' },</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>443</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="2"/>
+        <v>'Grenadine (Гренадин)'</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Grenadine (Гренадин)' },</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Grenadine (Гренадин)', name: 'Grenadine (Гренадин)' },</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" t="s">
+        <v>444</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="2"/>
+        <v>'Harvest Berry (Лесные ягоды)'</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Harvest Berry (Лесные ягоды)' },</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Harvest Berry (Лесные ягоды)', name: 'Harvest Berry (Лесные ягоды)' },</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" t="s">
+        <v>445</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="2"/>
+        <v>'Hazelnut (Лесной орех)'</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Hazelnut (Лесной орех)' },</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Hazelnut (Лесной орех)', name: 'Hazelnut (Лесной орех)' },</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" t="s">
+        <v>446</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="2"/>
+        <v>'Honeydew Melon (Медовая дыня)'</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Honeydew Melon (Медовая дыня)' },</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Honeydew Melon (Медовая дыня)', name: 'Honeydew Melon (Медовая дыня)' },</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" t="s">
+        <v>499</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="2"/>
+        <v>'Italian Lemon Sicily (Сицилийский лимон)'</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Italian Lemon Sicily (Сицилийский лимон)' },</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Italian Lemon Sicily (Сицилийский лимон)', name: 'Italian Lemon Sicily (Сицилийский лимон)' },</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" t="s">
+        <v>500</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="2"/>
+        <v>'Jelly Candy (Конфеты из желе)'</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Jelly Candy (Конфеты из желе)' },</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Jelly Candy (Конфеты из желе)', name: 'Jelly Candy (Конфеты из желе)' },</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" t="s">
+        <v>447</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="2"/>
+        <v>'Jelly Candys (Конфеты желе)'</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Jelly Candys (Конфеты желе)' },</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Jelly Candys (Конфеты желе)', name: 'Jelly Candys (Конфеты желе)' },</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" t="s">
+        <v>448</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="2"/>
+        <v>'Juicy Lemon (Сок лимона)'</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Juicy Lemon (Сок лимона)' },</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Juicy Lemon (Сок лимона)', name: 'Juicy Lemon (Сок лимона)' },</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" t="s">
+        <v>449</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="2"/>
+        <v>'Juicy Orange (Сочный апельсин)'</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Juicy Orange (Сочный апельсин)' },</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Juicy Orange (Сочный апельсин)', name: 'Juicy Orange (Сочный апельсин)' },</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" t="s">
+        <v>450</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="2"/>
+        <v>'Juicy Peach (Сочный персик)'</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Juicy Peach (Сочный персик)' },</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Juicy Peach (Сочный персик)', name: 'Juicy Peach (Сочный персик)' },</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>451</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="2"/>
+        <v>'Kiwi (Киви)'</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Kiwi (Киви)' },</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Kiwi (Киви)', name: 'Kiwi (Киви)' },</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>452</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="2"/>
+        <v>'Kiwi Strawberry (Киви и клубника)'</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Kiwi Strawberry (Киви и клубника)' },</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Kiwi Strawberry (Киви и клубника)', name: 'Kiwi Strawberry (Киви и клубника)' },</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>453</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="2"/>
+        <v>'Lemon Lime (Лимон-лайм)'</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Lemon Lime (Лимон-лайм)' },</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Lemon Lime (Лимон-лайм)', name: 'Lemon Lime (Лимон-лайм)' },</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>501</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="2"/>
+        <v>'Lemon Meringue Pie (Лимонный пирог с безе)'</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Lemon Meringue Pie (Лимонный пирог с безе)' },</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Lemon Meringue Pie (Лимонный пирог с безе)', name: 'Lemon Meringue Pie (Лимонный пирог с безе)' },</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" t="s">
+        <v>454</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="2"/>
+        <v>'Maple (Pancake Syrup) (Кленовый сироп)'</v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Maple (Pancake Syrup) (Кленовый сироп)' },</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Maple (Pancake Syrup) (Кленовый сироп)', name: 'Maple (Pancake Syrup) (Кленовый сироп)' },</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" t="s">
+        <v>455</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="2"/>
+        <v>'Milk Chocolate Toffee (Шоколаный тоффи)'</v>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Milk Chocolate Toffee (Шоколаный тоффи)' },</v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Milk Chocolate Toffee (Шоколаный тоффи)', name: 'Milk Chocolate Toffee (Шоколаный тоффи)' },</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" t="s">
+        <v>502</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="2"/>
+        <v>'New York Cheesecake (New York чизкейк)'</v>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'New York Cheesecake (New York чизкейк)' },</v>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'New York Cheesecake (New York чизкейк)', name: 'New York Cheesecake (New York чизкейк)' },</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" t="s">
+        <v>456</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="2"/>
+        <v>'New York Cheesecake v2 (New York чизкейк v2)'</v>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'New York Cheesecake v2 (New York чизкейк v2)' },</v>
+      </c>
+      <c r="L60" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'New York Cheesecake v2 (New York чизкейк v2)', name: 'New York Cheesecake v2 (New York чизкейк v2)' },</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" t="s">
+        <v>457</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="2"/>
+        <v>'Orange Creamsicle (Апельсиновое мороженное)'</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Orange Creamsicle (Апельсиновое мороженное)' },</v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Orange Creamsicle (Апельсиновое мороженное)', name: 'Orange Creamsicle (Апельсиновое мороженное)' },</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" t="s">
+        <v>458</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="2"/>
+        <v>'Orange Mango (Апельсин и манго)'</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Orange Mango (Апельсин и манго)' },</v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Orange Mango (Апельсин и манго)', name: 'Orange Mango (Апельсин и манго)' },</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" t="s">
+        <v>459</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="2"/>
+        <v>'Passion Fruit (Маракуйя)'</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Passion Fruit (Маракуйя)' },</v>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Passion Fruit (Маракуйя)', name: 'Passion Fruit (Маракуйя)' },</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" t="s">
+        <v>460</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="2"/>
+        <v>'Peach w/Stevia (Персик и стевия)'</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Peach w/Stevia (Персик и стевия)' },</v>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Peach w/Stevia (Персик и стевия)', name: 'Peach w/Stevia (Персик и стевия)' },</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" t="s">
+        <v>461</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="2"/>
+        <v>'Peaches and Cream (Персики в крему)'</v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Peaches and Cream (Персики в крему)' },</v>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Peaches and Cream (Персики в крему)', name: 'Peaches and Cream (Персики в крему)' },</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" t="s">
+        <v>462</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="2"/>
+        <v>'Peaches and Cream v2 (Персики в крему v2)'</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="3"/>
+        <v>{name: 'Peaches and Cream v2 (Персики в крему v2)' },</v>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="4"/>
+        <v>{id: 'Peaches and Cream v2 (Персики в крему v2)', name: 'Peaches and Cream v2 (Персики в крему v2)' },</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" t="s">
+        <v>463</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B94" si="5">CONCATENATE("'",A67,"'")</f>
+        <v>'Peanut Butter V2 (Арахисовое масло (версия 2))'</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K94" si="6">CONCATENATE($F$1,$H$1,B67,$J$1)</f>
+        <v>{name: 'Peanut Butter V2 (Арахисовое масло (версия 2))' },</v>
+      </c>
+      <c r="L67" t="str">
+        <f t="shared" ref="L67:L94" si="7">CONCATENATE($F$1,$G$1,B67,$H$2,$H$1,B67,$J$1)</f>
+        <v>{id: 'Peanut Butter V2 (Арахисовое масло (версия 2))', name: 'Peanut Butter V2 (Арахисовое масло (версия 2))' },</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" t="s">
+        <v>464</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="5"/>
+        <v>'Pear Flavor (Груша)'</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Pear Flavor (Груша)' },</v>
+      </c>
+      <c r="L68" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Pear Flavor (Груша)', name: 'Pear Flavor (Груша)' },</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" t="s">
+        <v>465</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="5"/>
+        <v>'Pink Lemonades (Лимонад)'</v>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Pink Lemonades (Лимонад)' },</v>
+      </c>
+      <c r="L69" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Pink Lemonades (Лимонад)', name: 'Pink Lemonades (Лимонад)' },</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" t="s">
+        <v>466</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="5"/>
+        <v>'Pomegranate V2 (Гранат 2)'</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Pomegranate V2 (Гранат 2)' },</v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Pomegranate V2 (Гранат 2)', name: 'Pomegranate V2 (Гранат 2)' },</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" t="s">
+        <v>467</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="5"/>
+        <v>'Raspberry (Малина)'</v>
+      </c>
+      <c r="K71" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Raspberry (Малина)' },</v>
+      </c>
+      <c r="L71" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Raspberry (Малина)', name: 'Raspberry (Малина)' },</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" t="s">
+        <v>468</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="5"/>
+        <v>'Raspberry V2 (Малина 2)'</v>
+      </c>
+      <c r="K72" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Raspberry V2 (Малина 2)' },</v>
+      </c>
+      <c r="L72" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Raspberry V2 (Малина 2)', name: 'Raspberry V2 (Малина 2)' },</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" t="s">
+        <v>503</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="5"/>
+        <v>'Simply Vanilla (Ваниль)'</v>
+      </c>
+      <c r="K73" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Simply Vanilla (Ваниль)' },</v>
+      </c>
+      <c r="L73" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Simply Vanilla (Ваниль)', name: 'Simply Vanilla (Ваниль)' },</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" t="s">
+        <v>469</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="5"/>
+        <v>'Strawberries and Cream ( Клубника в сливках)'</v>
+      </c>
+      <c r="K74" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Strawberries and Cream ( Клубника в сливках)' },</v>
+      </c>
+      <c r="L74" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Strawberries and Cream ( Клубника в сливках)', name: 'Strawberries and Cream ( Клубника в сливках)' },</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" t="s">
+        <v>470</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="5"/>
+        <v>'Strawberry Taffys (Клубничный тэфи)'</v>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Strawberry Taffys (Клубничный тэфи)' },</v>
+      </c>
+      <c r="L75" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Strawberry Taffys (Клубничный тэфи)', name: 'Strawberry Taffys (Клубничный тэфи)' },</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" t="s">
+        <v>471</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sugar Cookie v2 (Сахарное печенье v2)'</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sugar Cookie v2 (Сахарное печенье v2)' },</v>
+      </c>
+      <c r="L76" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sugar Cookie v2 (Сахарное печенье v2)', name: 'Sugar Cookie v2 (Сахарное печенье v2)' },</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" t="s">
+        <v>472</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="5"/>
+        <v>'Super Sweet Sucralose Sweetener (Подсластитель)'</v>
+      </c>
+      <c r="K77" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Super Sweet Sucralose Sweetener (Подсластитель)' },</v>
+      </c>
+      <c r="L77" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Super Sweet Sucralose Sweetener (Подсластитель)', name: 'Super Sweet Sucralose Sweetener (Подсластитель)' },</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" t="s">
+        <v>473</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Cream (Сладкий крем)'</v>
+      </c>
+      <c r="K78" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Cream (Сладкий крем)' },</v>
+      </c>
+      <c r="L78" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Cream (Сладкий крем)', name: 'Sweet Cream (Сладкий крем)' },</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" t="s">
+        <v>474</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Lychee (Сладкий личи)'</v>
+      </c>
+      <c r="K79" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Lychee (Сладкий личи)' },</v>
+      </c>
+      <c r="L79" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Lychee (Сладкий личи)', name: 'Sweet Lychee (Сладкий личи)' },</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" t="s">
+        <v>475</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Mango (Сладкий манго)'</v>
+      </c>
+      <c r="K80" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Mango (Сладкий манго)' },</v>
+      </c>
+      <c r="L80" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Mango (Сладкий манго)', name: 'Sweet Mango (Сладкий манго)' },</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" t="s">
+        <v>504</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Strawberry (Сладкая клубника)'</v>
+      </c>
+      <c r="K81" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Strawberry (Сладкая клубника)' },</v>
+      </c>
+      <c r="L81" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Strawberry (Сладкая клубника)', name: 'Sweet Strawberry (Сладкая клубника)' },</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" t="s">
+        <v>505</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Strawberry RF (Сладкая клубника РФ)'</v>
+      </c>
+      <c r="K82" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Strawberry RF (Сладкая клубника РФ)' },</v>
+      </c>
+      <c r="L82" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Strawberry RF (Сладкая клубника РФ)', name: 'Sweet Strawberry RF (Сладкая клубника РФ)' },</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" t="s">
+        <v>476</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Tangerine (Сладкий мандарин)'</v>
+      </c>
+      <c r="K83" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Tangerine (Сладкий мандарин)' },</v>
+      </c>
+      <c r="L83" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Tangerine (Сладкий мандарин)', name: 'Sweet Tangerine (Сладкий мандарин)' },</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" t="s">
+        <v>477</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Tangerine Rf (Сладкий мандарин)'</v>
+      </c>
+      <c r="K84" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Tangerine Rf (Сладкий мандарин)' },</v>
+      </c>
+      <c r="L84" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Tangerine Rf (Сладкий мандарин)', name: 'Sweet Tangerine Rf (Сладкий мандарин)' },</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" t="s">
+        <v>478</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Tea (Сладкий чай)'</v>
+      </c>
+      <c r="K85" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Tea (Сладкий чай)' },</v>
+      </c>
+      <c r="L85" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Tea (Сладкий чай)', name: 'Sweet Tea (Сладкий чай)' },</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86" t="s">
+        <v>479</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="5"/>
+        <v>'Sweet Watermelon (Сладкий арбуз)'</v>
+      </c>
+      <c r="K86" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Sweet Watermelon (Сладкий арбуз)' },</v>
+      </c>
+      <c r="L86" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Sweet Watermelon (Сладкий арбуз)', name: 'Sweet Watermelon (Сладкий арбуз)' },</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" t="s">
+        <v>480</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="5"/>
+        <v>'Vanilla Bean Ice Cream (Ванильное мороженное)'</v>
+      </c>
+      <c r="K87" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Vanilla Bean Ice Cream (Ванильное мороженное)' },</v>
+      </c>
+      <c r="L87" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Vanilla Bean Ice Cream (Ванильное мороженное)', name: 'Vanilla Bean Ice Cream (Ванильное мороженное)' },</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88" t="s">
+        <v>481</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="5"/>
+        <v>'Vanilla Cupcake V2 (Ванильный пирог)'</v>
+      </c>
+      <c r="K88" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Vanilla Cupcake V2 (Ванильный пирог)' },</v>
+      </c>
+      <c r="L88" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Vanilla Cupcake V2 (Ванильный пирог)', name: 'Vanilla Cupcake V2 (Ванильный пирог)' },</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89" t="s">
+        <v>482</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="5"/>
+        <v>'Vanilla Custard (Ванильный кастард)'</v>
+      </c>
+      <c r="K89" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Vanilla Custard (Ванильный кастард)' },</v>
+      </c>
+      <c r="L89" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Vanilla Custard (Ванильный кастард)', name: 'Vanilla Custard (Ванильный кастард)' },</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" t="s">
+        <v>506</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="5"/>
+        <v>'Vanilla Custard V2 (Ванильный крем v2)'</v>
+      </c>
+      <c r="K90" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Vanilla Custard V2 (Ванильный крем v2)' },</v>
+      </c>
+      <c r="L90" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Vanilla Custard V2 (Ванильный крем v2)', name: 'Vanilla Custard V2 (Ванильный крем v2)' },</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91" t="s">
+        <v>483</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="5"/>
+        <v>'Vanilla Whipped Cream (Ванильные взбитые сливки)'</v>
+      </c>
+      <c r="K91" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Vanilla Whipped Cream (Ванильные взбитые сливки)' },</v>
+      </c>
+      <c r="L91" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Vanilla Whipped Cream (Ванильные взбитые сливки)', name: 'Vanilla Whipped Cream (Ванильные взбитые сливки)' },</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92" t="s">
+        <v>484</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="5"/>
+        <v>'Waffle (Вафли)'</v>
+      </c>
+      <c r="K92" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Waffle (Вафли)' },</v>
+      </c>
+      <c r="L92" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Waffle (Вафли)', name: 'Waffle (Вафли)' },</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" t="s">
+        <v>507</v>
+      </c>
+      <c r="B93" t="str">
+        <f t="shared" si="5"/>
+        <v>'Wild Cherry (Дикая вишня)'</v>
+      </c>
+      <c r="K93" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Wild Cherry (Дикая вишня)' },</v>
+      </c>
+      <c r="L93" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Wild Cherry (Дикая вишня)', name: 'Wild Cherry (Дикая вишня)' },</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" t="s">
+        <v>485</v>
+      </c>
+      <c r="B94" t="str">
+        <f t="shared" si="5"/>
+        <v>'Yellow Peach (Желтый персик)'</v>
+      </c>
+      <c r="K94" t="str">
+        <f t="shared" si="6"/>
+        <v>{name: 'Yellow Peach (Желтый персик)' },</v>
+      </c>
+      <c r="L94" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Yellow Peach (Желтый персик)', name: 'Yellow Peach (Желтый персик)' },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B1" t="str">
+        <f>CONCATENATE("'",A1,"'")</f>
+        <v>'Apple Pie (Яблочный Пирог)'</v>
+      </c>
+      <c r="F1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1" t="s">
+        <v>411</v>
+      </c>
+      <c r="J1" t="s">
+        <v>412</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE($F$1,$H$1,B1,$J$1)</f>
+        <v>{name: 'Apple Pie (Яблочный Пирог)' },</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE($F$1,$G$1,B1,$H$2,$H$1,B1,$J$1)</f>
+        <v>{id: 'Apple Pie (Яблочный Пирог)', name: 'Apple Pie (Яблочный Пирог)' },</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B39" si="0">CONCATENATE("'",A2,"'")</f>
+        <v>'Bilberry (Черника)'</v>
+      </c>
+      <c r="H2" t="s">
+        <v>413</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K39" si="1">CONCATENATE($F$1,$H$1,B2,$J$1)</f>
+        <v>{name: 'Bilberry (Черника)' },</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L39" si="2">CONCATENATE($F$1,$G$1,B2,$H$2,$H$1,B2,$J$1)</f>
+        <v>{id: 'Bilberry (Черника)', name: 'Bilberry (Черника)' },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>510</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>'Biscotto Cookie (Овсяное Печенье)'</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Biscotto Cookie (Овсяное Печенье)' },</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Biscotto Cookie (Овсяное Печенье)', name: 'Biscotto Cookie (Овсяное Печенье)' },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>'Blackberry (Ежевика)'</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Blackberry (Ежевика)' },</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Blackberry (Ежевика)', name: 'Blackberry (Ежевика)' },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>'Blackcurrant (Черная Смородина)'</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Blackcurrant (Черная Смородина)' },</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Blackcurrant (Черная Смородина)', name: 'Blackcurrant (Черная Смородина)' },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>512</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>'Caramel (Карамель)'</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Caramel (Карамель)' },</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Caramel (Карамель)', name: 'Caramel (Карамель)' },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>513</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Champagne (Шампанское)'</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Champagne (Шампанское)' },</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Champagne (Шампанское)', name: 'Champagne (Шампанское)' },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>514</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>'Cherry (Вишня)'</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Cherry (Вишня)' },</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Cherry (Вишня)', name: 'Cherry (Вишня)' },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>515</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>'Citrus Mix (Цитрусовый Микс)'</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Citrus Mix (Цитрусовый Микс)' },</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Citrus Mix (Цитрусовый Микс)', name: 'Citrus Mix (Цитрусовый Микс)' },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>516</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>'Classic Vanilla (Ваниль)'</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Classic Vanilla (Ваниль)' },</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Classic Vanilla (Ваниль)', name: 'Classic Vanilla (Ваниль)' },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>496</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>'Coconut (Кокос)'</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Coconut (Кокос)' },</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Coconut (Кокос)', name: 'Coconut (Кокос)' },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>429</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>'Cola (Кола)'</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Cola (Кола)' },</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Cola (Кола)', name: 'Cola (Кола)' },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>517</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Custard Cream (Заварной Крем)'</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Custard Cream (Заварной Крем)' },</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Custard Cream (Заварной Крем)', name: 'Custard Cream (Заварной Крем)' },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>518</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>'Forest Fruit Mix (Фруктовый Микс)'</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Forest Fruit Mix (Фруктовый Микс)' },</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Forest Fruit Mix (Фруктовый Микс)', name: 'Forest Fruit Mix (Фруктовый Микс)' },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>519</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>'Fuji Apple (Яблоко Fuji)'</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Fuji Apple (Яблоко Fuji)' },</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Fuji Apple (Яблоко Fuji)', name: 'Fuji Apple (Яблоко Fuji)' },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>520</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>'Green Tea (Зеленый Чай)'</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Green Tea (Зеленый Чай)' },</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Green Tea (Зеленый Чай)', name: 'Green Tea (Зеленый Чай)' },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>521</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>'Hazelnut (Лесной Орех)'</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Hazelnut (Лесной Орех)' },</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Hazelnut (Лесной Орех)', name: 'Hazelnut (Лесной Орех)' },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>451</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>'Kiwi (Киви)'</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Kiwi (Киви)' },</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Kiwi (Киви)', name: 'Kiwi (Киви)' },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>522</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>'Lemon Sicily (Лимон Сицилийский)'</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Lemon Sicily (Лимон Сицилийский)' },</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Lemon Sicily (Лимон Сицилийский)', name: 'Lemon Sicily (Лимон Сицилийский)' },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>523</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>'Lime Tahity Distilled (Лайм)'</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Lime Tahity Distilled (Лайм)' },</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Lime Tahity Distilled (Лайм)', name: 'Lime Tahity Distilled (Лайм)' },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>524</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>'Mandarin (Мандарин)'</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Mandarin (Мандарин)' },</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Mandarin (Мандарин)', name: 'Mandarin (Мандарин)' },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>525</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>'Mango (Манго)'</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Mango (Манго)' },</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Mango (Манго)', name: 'Mango (Манго)' },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>526</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>'Marshmallow (Зефир)'</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Marshmallow (Зефир)' },</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Marshmallow (Зефир)', name: 'Marshmallow (Зефир)' },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>527</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>'Maxx Blend (Табак Maxx Blend)'</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Maxx Blend (Табак Maxx Blend)' },</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Maxx Blend (Табак Maxx Blend)', name: 'Maxx Blend (Табак Maxx Blend)' },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>528</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>'Melon Cantaloupe (Мускусная Дыня)'</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Melon Cantaloupe (Мускусная Дыня)' },</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Melon Cantaloupe (Мускусная Дыня)', name: 'Melon Cantaloupe (Мускусная Дыня)' },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>529</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Menthol (Ментол)'</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Menthol (Ментол)' },</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Menthol (Ментол)', name: 'Menthol (Ментол)' },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>530</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>'Meringue (Безе)'</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Meringue (Безе)' },</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Meringue (Безе)', name: 'Meringue (Безе)' },</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>531</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>'Nonna’s Cake (Пирог Нонны)'</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Nonna’s Cake (Пирог Нонны)' },</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Nonna’s Cake (Пирог Нонны)', name: 'Nonna’s Cake (Пирог Нонны)' },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>532</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>'Orange (Апельсин)'</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Orange (Апельсин)' },</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Orange (Апельсин)', name: 'Orange (Апельсин)' },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>533</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>'Passionfruit (Маракуйя)'</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Passionfruit (Маракуйя)' },</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Passionfruit (Маракуйя)', name: 'Passionfruit (Маракуйя)' },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>467</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>'Raspberry (Малина)'</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Raspberry (Малина)' },</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Raspberry (Малина)', name: 'Raspberry (Малина)' },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>534</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>'Soho (Табак Soho)'</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Soho (Табак Soho)' },</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Soho (Табак Soho)', name: 'Soho (Табак Soho)' },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>535</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>'Spearmint (Мятная Жвачка)'</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Spearmint (Мятная Жвачка)' },</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Spearmint (Мятная Жвачка)', name: 'Spearmint (Мятная Жвачка)' },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>536</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>'Stark Apple (Яблоко Красное)'</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Stark Apple (Яблоко Красное)' },</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Stark Apple (Яблоко Красное)', name: 'Stark Apple (Яблоко Красное)' },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" t="s">
+        <v>537</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>'Strawberry (Клубника)'</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Strawberry (Клубника)' },</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Strawberry (Клубника)', name: 'Strawberry (Клубника)' },</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" t="s">
+        <v>538</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>'Virginia (Табак Virginia)'</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Virginia (Табак Virginia)' },</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Virginia (Табак Virginia)', name: 'Virginia (Табак Virginia)' },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" t="s">
+        <v>539</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>'Watermelon (Арбуз)'</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Watermelon (Арбуз)' },</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Watermelon (Арбуз)', name: 'Watermelon (Арбуз)' },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>540</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>'White Peach (Белый Персик)'</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'White Peach (Белый Персик)' },</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'White Peach (Белый Персик)', name: 'White Peach (Белый Персик)' },</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" t="s">
+        <v>541</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>'Yogurt (Йогурт)'</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>{name: 'Yogurt (Йогурт)' },</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="2"/>
+        <v>{id: 'Yogurt (Йогурт)', name: 'Yogurt (Йогурт)' },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Everyhting works now - deselection highlight when clicking cross button in right side of slider
</commit_message>
<xml_diff>
--- a/info/список ароматизаторов.xlsx
+++ b/info/список ароматизаторов.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -8694,7 +8694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
@@ -12671,7 +12671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1:M94"/>
     </sheetView>
   </sheetViews>
@@ -12711,8 +12711,8 @@
         <v>{name: 'Apple Pie (Яблочный пирог)' },</v>
       </c>
       <c r="M1" t="str">
-        <f>CONCATENATE($G$1,$H$1,A1,$I$2,$I$1,C1,$K$1)</f>
-        <v>{id: 2001, name: 'Apple Pie (Яблочный пирог)' },</v>
+        <f>CONCATENATE($G$1,$H$1,A1,$I$2,$I$1,C1,$I$2,$J$1,$K$1)</f>
+        <v>{id: 2001, name: 'Apple Pie (Яблочный пирог)', isSelected: false },</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -12734,8 +12734,8 @@
         <v>{name: 'Apple Pie V2 (Яблочный пирог 2)' },</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M65" si="1">CONCATENATE($G$1,$H$1,A2,$I$2,$I$1,C2,$K$1)</f>
-        <v>{id: 2002, name: 'Apple Pie V2 (Яблочный пирог 2)' },</v>
+        <f t="shared" ref="M2:M65" si="1">CONCATENATE($G$1,$H$1,A2,$I$2,$I$1,C2,$I$2,$J$1,$K$1)</f>
+        <v>{id: 2002, name: 'Apple Pie V2 (Яблочный пирог 2)', isSelected: false },</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -12755,7 +12755,7 @@
       </c>
       <c r="M3" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2003, name: 'Apricot (Абрикос)' },</v>
+        <v>{id: 2003, name: 'Apricot (Абрикос)', isSelected: false },</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -12775,7 +12775,7 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2004, name: 'Banana (Банан)' },</v>
+        <v>{id: 2004, name: 'Banana (Банан)', isSelected: false },</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -12795,7 +12795,7 @@
       </c>
       <c r="M5" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2005, name: 'Banana Split (Банановый сплит)' },</v>
+        <v>{id: 2005, name: 'Banana Split (Банановый сплит)', isSelected: false },</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -12815,7 +12815,7 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2006, name: 'Bavarian Cream (Баварский крем)' },</v>
+        <v>{id: 2006, name: 'Bavarian Cream (Баварский крем)', isSelected: false },</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -12835,7 +12835,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2007, name: 'Blackberry (Ежевика)' },</v>
+        <v>{id: 2007, name: 'Blackberry (Ежевика)', isSelected: false },</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -12855,7 +12855,7 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2008, name: 'Blueberry (Черника)' },</v>
+        <v>{id: 2008, name: 'Blueberry (Черника)', isSelected: false },</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -12875,7 +12875,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2009, name: 'Blueberry Cinnamon Crumble (Черничный пирог с корицей)' },</v>
+        <v>{id: 2009, name: 'Blueberry Cinnamon Crumble (Черничный пирог с корицей)', isSelected: false },</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -12895,7 +12895,7 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2010, name: 'Blueberry Jam (Черничное варенье)' },</v>
+        <v>{id: 2010, name: 'Blueberry Jam (Черничное варенье)', isSelected: false },</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -12915,7 +12915,7 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2011, name: 'Blueberry Pomegranate (Черника и гранат)' },</v>
+        <v>{id: 2011, name: 'Blueberry Pomegranate (Черника и гранат)', isSelected: false },</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -12935,7 +12935,7 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2012, name: 'Boston Cream Pie V2 (Бостонский кремовый пирог)' },</v>
+        <v>{id: 2012, name: 'Boston Cream Pie V2 (Бостонский кремовый пирог)', isSelected: false },</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -12955,7 +12955,7 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2013, name: 'Bubble Gum (Жвачка)' },</v>
+        <v>{id: 2013, name: 'Bubble Gum (Жвачка)', isSelected: false },</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -12975,7 +12975,7 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2014, name: 'Butter Cream (Крем)' },</v>
+        <v>{id: 2014, name: 'Butter Cream (Крем)', isSelected: false },</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -12995,7 +12995,7 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2015, name: 'Cake Batter (Тесто для кекса)' },</v>
+        <v>{id: 2015, name: 'Cake Batter (Тесто для кекса)', isSelected: false },</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -13015,7 +13015,7 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2016, name: 'Cantaloupe (Мускусная дыня)' },</v>
+        <v>{id: 2016, name: 'Cantaloupe (Мускусная дыня)', isSelected: false },</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -13035,7 +13035,7 @@
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2017, name: 'Cappuccino (Каппучино)' },</v>
+        <v>{id: 2017, name: 'Cappuccino (Каппучино)', isSelected: false },</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -13055,7 +13055,7 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2018, name: 'Caramel V2 (Карамель 2)' },</v>
+        <v>{id: 2018, name: 'Caramel V2 (Карамель 2)', isSelected: false },</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -13075,7 +13075,7 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2019, name: 'Cereal 27 (Кукурузные хлопья)' },</v>
+        <v>{id: 2019, name: 'Cereal 27 (Кукурузные хлопья)', isSelected: false },</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -13095,7 +13095,7 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2020, name: 'Cherry (Wild) w/Stevia (Дикая вишня и стевия)' },</v>
+        <v>{id: 2020, name: 'Cherry (Wild) w/Stevia (Дикая вишня и стевия)', isSelected: false },</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -13115,7 +13115,7 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2021, name: 'Chocolate Coconut Almond (Шоколад кокос миндаль)' },</v>
+        <v>{id: 2021, name: 'Chocolate Coconut Almond (Шоколад кокос миндаль)', isSelected: false },</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -13135,7 +13135,7 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2022, name: 'Chocolate Glazed Doughnut (Глазированный шаколадный пончик)' },</v>
+        <v>{id: 2022, name: 'Chocolate Glazed Doughnut (Глазированный шаколадный пончик)', isSelected: false },</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -13155,7 +13155,7 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2023, name: 'Chocolate Raspberry (Малина с шоколадом)' },</v>
+        <v>{id: 2023, name: 'Chocolate Raspberry (Малина с шоколадом)', isSelected: false },</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -13175,7 +13175,7 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2024, name: 'Churro (Чуррос)' },</v>
+        <v>{id: 2024, name: 'Churro (Чуррос)', isSelected: false },</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -13195,7 +13195,7 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2025, name: 'Cinnamon Danish Swirl V2 (Датский завиток с корицей 2)' },</v>
+        <v>{id: 2025, name: 'Cinnamon Danish Swirl V2 (Датский завиток с корицей 2)', isSelected: false },</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -13215,7 +13215,7 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2026, name: 'Coconut (Кокос)' },</v>
+        <v>{id: 2026, name: 'Coconut (Кокос)', isSelected: false },</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -13235,7 +13235,7 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2027, name: 'Cola (Кола)' },</v>
+        <v>{id: 2027, name: 'Cola (Кола)', isSelected: false },</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -13255,7 +13255,7 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2028, name: 'Concord Grape w/Stevia (Конкорд и стевия)' },</v>
+        <v>{id: 2028, name: 'Concord Grape w/Stevia (Конкорд и стевия)', isSelected: false },</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -13275,7 +13275,7 @@
       </c>
       <c r="M29" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2029, name: 'Cool Mint (Мятная свежесть)' },</v>
+        <v>{id: 2029, name: 'Cool Mint (Мятная свежесть)', isSelected: false },</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -13295,7 +13295,7 @@
       </c>
       <c r="M30" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2030, name: 'Cranberry (Клюква)' },</v>
+        <v>{id: 2030, name: 'Cranberry (Клюква)', isSelected: false },</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -13315,7 +13315,7 @@
       </c>
       <c r="M31" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2031, name: 'Creamy Yogurt (Кремовый йогурт)' },</v>
+        <v>{id: 2031, name: 'Creamy Yogurt (Кремовый йогурт)', isSelected: false },</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -13335,7 +13335,7 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2032, name: 'Double Apple (Двойное яблоко)' },</v>
+        <v>{id: 2032, name: 'Double Apple (Двойное яблоко)', isSelected: false },</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -13355,7 +13355,7 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2033, name: 'Double Watermelon (Двойной арбуз)' },</v>
+        <v>{id: 2033, name: 'Double Watermelon (Двойной арбуз)', isSelected: false },</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -13375,7 +13375,7 @@
       </c>
       <c r="M34" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2034, name: 'Dragon Fruit (Драгонфрут)' },</v>
+        <v>{id: 2034, name: 'Dragon Fruit (Драгонфрут)', isSelected: false },</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -13395,7 +13395,7 @@
       </c>
       <c r="M35" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2035, name: 'French Vanilla (Французкая ваниль)' },</v>
+        <v>{id: 2035, name: 'French Vanilla (Французкая ваниль)', isSelected: false },</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -13415,7 +13415,7 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2036, name: 'Funnel Cake (Торт "Муравейник")' },</v>
+        <v>{id: 2036, name: 'Funnel Cake (Торт "Муравейник")', isSelected: false },</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -13435,7 +13435,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2037, name: 'Glazed Doughnut (Глазированный пончик)' },</v>
+        <v>{id: 2037, name: 'Glazed Doughnut (Глазированный пончик)', isSelected: false },</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -13455,7 +13455,7 @@
       </c>
       <c r="M38" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2038, name: 'Golden Pineapple (Золотой ананас)' },</v>
+        <v>{id: 2038, name: 'Golden Pineapple (Золотой ананас)', isSelected: false },</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -13475,7 +13475,7 @@
       </c>
       <c r="M39" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2039, name: 'Graham Cracker V2 (Грэхем крекер 2)' },</v>
+        <v>{id: 2039, name: 'Graham Cracker V2 (Грэхем крекер 2)', isSelected: false },</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -13495,7 +13495,7 @@
       </c>
       <c r="M40" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2040, name: 'Grapefruit (Грейпфрут)' },</v>
+        <v>{id: 2040, name: 'Grapefruit (Грейпфрут)', isSelected: false },</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -13515,7 +13515,7 @@
       </c>
       <c r="M41" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2041, name: 'Greek Yogurt (Греческий йогурт)' },</v>
+        <v>{id: 2041, name: 'Greek Yogurt (Греческий йогурт)', isSelected: false },</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -13535,7 +13535,7 @@
       </c>
       <c r="M42" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2042, name: 'Green Apple (Зеленое яблоко)' },</v>
+        <v>{id: 2042, name: 'Green Apple (Зеленое яблоко)', isSelected: false },</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -13555,7 +13555,7 @@
       </c>
       <c r="M43" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2043, name: 'Grenadine (Гренадин)' },</v>
+        <v>{id: 2043, name: 'Grenadine (Гренадин)', isSelected: false },</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -13575,7 +13575,7 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2044, name: 'Harvest Berry (Лесные ягоды)' },</v>
+        <v>{id: 2044, name: 'Harvest Berry (Лесные ягоды)', isSelected: false },</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -13595,7 +13595,7 @@
       </c>
       <c r="M45" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2045, name: 'Hazelnut (Лесной орех)' },</v>
+        <v>{id: 2045, name: 'Hazelnut (Лесной орех)', isSelected: false },</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -13615,7 +13615,7 @@
       </c>
       <c r="M46" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2046, name: 'Honeydew Melon (Медовая дыня)' },</v>
+        <v>{id: 2046, name: 'Honeydew Melon (Медовая дыня)', isSelected: false },</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -13635,7 +13635,7 @@
       </c>
       <c r="M47" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2047, name: 'Italian Lemon Sicily (Сицилийский лимон)' },</v>
+        <v>{id: 2047, name: 'Italian Lemon Sicily (Сицилийский лимон)', isSelected: false },</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -13655,7 +13655,7 @@
       </c>
       <c r="M48" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2048, name: 'Jelly Candy (Конфеты из желе)' },</v>
+        <v>{id: 2048, name: 'Jelly Candy (Конфеты из желе)', isSelected: false },</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -13675,7 +13675,7 @@
       </c>
       <c r="M49" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2049, name: 'Jelly Candys (Конфеты желе)' },</v>
+        <v>{id: 2049, name: 'Jelly Candys (Конфеты желе)', isSelected: false },</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -13695,7 +13695,7 @@
       </c>
       <c r="M50" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2050, name: 'Juicy Lemon (Сок лимона)' },</v>
+        <v>{id: 2050, name: 'Juicy Lemon (Сок лимона)', isSelected: false },</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -13715,7 +13715,7 @@
       </c>
       <c r="M51" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2051, name: 'Juicy Orange (Сочный апельсин)' },</v>
+        <v>{id: 2051, name: 'Juicy Orange (Сочный апельсин)', isSelected: false },</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -13735,7 +13735,7 @@
       </c>
       <c r="M52" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2052, name: 'Juicy Peach (Сочный персик)' },</v>
+        <v>{id: 2052, name: 'Juicy Peach (Сочный персик)', isSelected: false },</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -13755,7 +13755,7 @@
       </c>
       <c r="M53" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2053, name: 'Kiwi (Киви)' },</v>
+        <v>{id: 2053, name: 'Kiwi (Киви)', isSelected: false },</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -13775,7 +13775,7 @@
       </c>
       <c r="M54" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2054, name: 'Kiwi Strawberry (Киви и клубника)' },</v>
+        <v>{id: 2054, name: 'Kiwi Strawberry (Киви и клубника)', isSelected: false },</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -13795,7 +13795,7 @@
       </c>
       <c r="M55" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2055, name: 'Lemon Lime (Лимон-лайм)' },</v>
+        <v>{id: 2055, name: 'Lemon Lime (Лимон-лайм)', isSelected: false },</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -13815,7 +13815,7 @@
       </c>
       <c r="M56" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2056, name: 'Lemon Meringue Pie (Лимонный пирог с безе)' },</v>
+        <v>{id: 2056, name: 'Lemon Meringue Pie (Лимонный пирог с безе)', isSelected: false },</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -13835,7 +13835,7 @@
       </c>
       <c r="M57" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2057, name: 'Maple (Pancake Syrup) (Кленовый сироп)' },</v>
+        <v>{id: 2057, name: 'Maple (Pancake Syrup) (Кленовый сироп)', isSelected: false },</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -13855,7 +13855,7 @@
       </c>
       <c r="M58" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2058, name: 'Milk Chocolate Toffee (Шоколаный тоффи)' },</v>
+        <v>{id: 2058, name: 'Milk Chocolate Toffee (Шоколаный тоффи)', isSelected: false },</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -13875,7 +13875,7 @@
       </c>
       <c r="M59" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2059, name: 'New York Cheesecake (New York чизкейк)' },</v>
+        <v>{id: 2059, name: 'New York Cheesecake (New York чизкейк)', isSelected: false },</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -13895,7 +13895,7 @@
       </c>
       <c r="M60" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2060, name: 'New York Cheesecake v2 (New York чизкейк v2)' },</v>
+        <v>{id: 2060, name: 'New York Cheesecake v2 (New York чизкейк v2)', isSelected: false },</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -13915,7 +13915,7 @@
       </c>
       <c r="M61" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2061, name: 'Orange Creamsicle (Апельсиновое мороженное)' },</v>
+        <v>{id: 2061, name: 'Orange Creamsicle (Апельсиновое мороженное)', isSelected: false },</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -13935,7 +13935,7 @@
       </c>
       <c r="M62" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2062, name: 'Orange Mango (Апельсин и манго)' },</v>
+        <v>{id: 2062, name: 'Orange Mango (Апельсин и манго)', isSelected: false },</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -13955,7 +13955,7 @@
       </c>
       <c r="M63" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2063, name: 'Passion Fruit (Маракуйя)' },</v>
+        <v>{id: 2063, name: 'Passion Fruit (Маракуйя)', isSelected: false },</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -13975,7 +13975,7 @@
       </c>
       <c r="M64" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2064, name: 'Peach w/Stevia (Персик и стевия)' },</v>
+        <v>{id: 2064, name: 'Peach w/Stevia (Персик и стевия)', isSelected: false },</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -13995,7 +13995,7 @@
       </c>
       <c r="M65" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 2065, name: 'Peaches and Cream (Персики в крему)' },</v>
+        <v>{id: 2065, name: 'Peaches and Cream (Персики в крему)', isSelected: false },</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -14014,8 +14014,8 @@
         <v>{name: 'Peaches and Cream v2 (Персики в крему v2)' },</v>
       </c>
       <c r="M66" t="str">
-        <f t="shared" ref="M66:M94" si="4">CONCATENATE($G$1,$H$1,A66,$I$2,$I$1,C66,$K$1)</f>
-        <v>{id: 2066, name: 'Peaches and Cream v2 (Персики в крему v2)' },</v>
+        <f t="shared" ref="M66:M94" si="4">CONCATENATE($G$1,$H$1,A66,$I$2,$I$1,C66,$I$2,$J$1,$K$1)</f>
+        <v>{id: 2066, name: 'Peaches and Cream v2 (Персики в крему v2)', isSelected: false },</v>
       </c>
     </row>
     <row r="67" spans="1:13">
@@ -14035,7 +14035,7 @@
       </c>
       <c r="M67" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2067, name: 'Peanut Butter V2 (Арахисовое масло (версия 2))' },</v>
+        <v>{id: 2067, name: 'Peanut Butter V2 (Арахисовое масло (версия 2))', isSelected: false },</v>
       </c>
     </row>
     <row r="68" spans="1:13">
@@ -14055,7 +14055,7 @@
       </c>
       <c r="M68" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2068, name: 'Pear Flavor (Груша)' },</v>
+        <v>{id: 2068, name: 'Pear Flavor (Груша)', isSelected: false },</v>
       </c>
     </row>
     <row r="69" spans="1:13">
@@ -14075,7 +14075,7 @@
       </c>
       <c r="M69" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2069, name: 'Pink Lemonades (Лимонад)' },</v>
+        <v>{id: 2069, name: 'Pink Lemonades (Лимонад)', isSelected: false },</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -14095,7 +14095,7 @@
       </c>
       <c r="M70" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2070, name: 'Pomegranate V2 (Гранат 2)' },</v>
+        <v>{id: 2070, name: 'Pomegranate V2 (Гранат 2)', isSelected: false },</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -14115,7 +14115,7 @@
       </c>
       <c r="M71" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2071, name: 'Raspberry (Малина)' },</v>
+        <v>{id: 2071, name: 'Raspberry (Малина)', isSelected: false },</v>
       </c>
     </row>
     <row r="72" spans="1:13">
@@ -14135,7 +14135,7 @@
       </c>
       <c r="M72" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2072, name: 'Raspberry V2 (Малина 2)' },</v>
+        <v>{id: 2072, name: 'Raspberry V2 (Малина 2)', isSelected: false },</v>
       </c>
     </row>
     <row r="73" spans="1:13">
@@ -14155,7 +14155,7 @@
       </c>
       <c r="M73" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2073, name: 'Simply Vanilla (Ваниль)' },</v>
+        <v>{id: 2073, name: 'Simply Vanilla (Ваниль)', isSelected: false },</v>
       </c>
     </row>
     <row r="74" spans="1:13">
@@ -14175,7 +14175,7 @@
       </c>
       <c r="M74" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2074, name: 'Strawberries and Cream ( Клубника в сливках)' },</v>
+        <v>{id: 2074, name: 'Strawberries and Cream ( Клубника в сливках)', isSelected: false },</v>
       </c>
     </row>
     <row r="75" spans="1:13">
@@ -14195,7 +14195,7 @@
       </c>
       <c r="M75" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2075, name: 'Strawberry Taffys (Клубничный тэфи)' },</v>
+        <v>{id: 2075, name: 'Strawberry Taffys (Клубничный тэфи)', isSelected: false },</v>
       </c>
     </row>
     <row r="76" spans="1:13">
@@ -14215,7 +14215,7 @@
       </c>
       <c r="M76" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2076, name: 'Sugar Cookie v2 (Сахарное печенье v2)' },</v>
+        <v>{id: 2076, name: 'Sugar Cookie v2 (Сахарное печенье v2)', isSelected: false },</v>
       </c>
     </row>
     <row r="77" spans="1:13">
@@ -14235,7 +14235,7 @@
       </c>
       <c r="M77" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2077, name: 'Super Sweet Sucralose Sweetener (Подсластитель)' },</v>
+        <v>{id: 2077, name: 'Super Sweet Sucralose Sweetener (Подсластитель)', isSelected: false },</v>
       </c>
     </row>
     <row r="78" spans="1:13">
@@ -14255,7 +14255,7 @@
       </c>
       <c r="M78" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2078, name: 'Sweet Cream (Сладкий крем)' },</v>
+        <v>{id: 2078, name: 'Sweet Cream (Сладкий крем)', isSelected: false },</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -14275,7 +14275,7 @@
       </c>
       <c r="M79" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2079, name: 'Sweet Lychee (Сладкий личи)' },</v>
+        <v>{id: 2079, name: 'Sweet Lychee (Сладкий личи)', isSelected: false },</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -14295,7 +14295,7 @@
       </c>
       <c r="M80" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2080, name: 'Sweet Mango (Сладкий манго)' },</v>
+        <v>{id: 2080, name: 'Sweet Mango (Сладкий манго)', isSelected: false },</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -14315,7 +14315,7 @@
       </c>
       <c r="M81" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2081, name: 'Sweet Strawberry (Сладкая клубника)' },</v>
+        <v>{id: 2081, name: 'Sweet Strawberry (Сладкая клубника)', isSelected: false },</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -14335,7 +14335,7 @@
       </c>
       <c r="M82" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2082, name: 'Sweet Strawberry RF (Сладкая клубника РФ)' },</v>
+        <v>{id: 2082, name: 'Sweet Strawberry RF (Сладкая клубника РФ)', isSelected: false },</v>
       </c>
     </row>
     <row r="83" spans="1:13">
@@ -14355,7 +14355,7 @@
       </c>
       <c r="M83" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2083, name: 'Sweet Tangerine (Сладкий мандарин)' },</v>
+        <v>{id: 2083, name: 'Sweet Tangerine (Сладкий мандарин)', isSelected: false },</v>
       </c>
     </row>
     <row r="84" spans="1:13">
@@ -14375,7 +14375,7 @@
       </c>
       <c r="M84" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2084, name: 'Sweet Tangerine Rf (Сладкий мандарин)' },</v>
+        <v>{id: 2084, name: 'Sweet Tangerine Rf (Сладкий мандарин)', isSelected: false },</v>
       </c>
     </row>
     <row r="85" spans="1:13">
@@ -14395,7 +14395,7 @@
       </c>
       <c r="M85" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2085, name: 'Sweet Tea (Сладкий чай)' },</v>
+        <v>{id: 2085, name: 'Sweet Tea (Сладкий чай)', isSelected: false },</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -14415,7 +14415,7 @@
       </c>
       <c r="M86" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2086, name: 'Sweet Watermelon (Сладкий арбуз)' },</v>
+        <v>{id: 2086, name: 'Sweet Watermelon (Сладкий арбуз)', isSelected: false },</v>
       </c>
     </row>
     <row r="87" spans="1:13">
@@ -14435,7 +14435,7 @@
       </c>
       <c r="M87" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2087, name: 'Vanilla Bean Ice Cream (Ванильное мороженное)' },</v>
+        <v>{id: 2087, name: 'Vanilla Bean Ice Cream (Ванильное мороженное)', isSelected: false },</v>
       </c>
     </row>
     <row r="88" spans="1:13">
@@ -14455,7 +14455,7 @@
       </c>
       <c r="M88" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2088, name: 'Vanilla Cupcake V2 (Ванильный пирог)' },</v>
+        <v>{id: 2088, name: 'Vanilla Cupcake V2 (Ванильный пирог)', isSelected: false },</v>
       </c>
     </row>
     <row r="89" spans="1:13">
@@ -14475,7 +14475,7 @@
       </c>
       <c r="M89" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2089, name: 'Vanilla Custard (Ванильный кастард)' },</v>
+        <v>{id: 2089, name: 'Vanilla Custard (Ванильный кастард)', isSelected: false },</v>
       </c>
     </row>
     <row r="90" spans="1:13">
@@ -14495,7 +14495,7 @@
       </c>
       <c r="M90" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2090, name: 'Vanilla Custard V2 (Ванильный крем v2)' },</v>
+        <v>{id: 2090, name: 'Vanilla Custard V2 (Ванильный крем v2)', isSelected: false },</v>
       </c>
     </row>
     <row r="91" spans="1:13">
@@ -14515,7 +14515,7 @@
       </c>
       <c r="M91" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2091, name: 'Vanilla Whipped Cream (Ванильные взбитые сливки)' },</v>
+        <v>{id: 2091, name: 'Vanilla Whipped Cream (Ванильные взбитые сливки)', isSelected: false },</v>
       </c>
     </row>
     <row r="92" spans="1:13">
@@ -14535,7 +14535,7 @@
       </c>
       <c r="M92" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2092, name: 'Waffle (Вафли)' },</v>
+        <v>{id: 2092, name: 'Waffle (Вафли)', isSelected: false },</v>
       </c>
     </row>
     <row r="93" spans="1:13">
@@ -14555,7 +14555,7 @@
       </c>
       <c r="M93" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2093, name: 'Wild Cherry (Дикая вишня)' },</v>
+        <v>{id: 2093, name: 'Wild Cherry (Дикая вишня)', isSelected: false },</v>
       </c>
     </row>
     <row r="94" spans="1:13">
@@ -14575,7 +14575,7 @@
       </c>
       <c r="M94" t="str">
         <f t="shared" si="4"/>
-        <v>{id: 2094, name: 'Yellow Peach (Желтый персик)' },</v>
+        <v>{id: 2094, name: 'Yellow Peach (Желтый персик)', isSelected: false },</v>
       </c>
     </row>
   </sheetData>
@@ -14588,7 +14588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:M39"/>
     </sheetView>
   </sheetViews>
@@ -14628,8 +14628,8 @@
         <v>{name: 'Apple Pie (Яблочный Пирог)' },</v>
       </c>
       <c r="M1" t="str">
-        <f>CONCATENATE($G$1,$H$1,A1,$I$2,$I$1,C1,$K$1)</f>
-        <v>{id: 3001, name: 'Apple Pie (Яблочный Пирог)' },</v>
+        <f>CONCATENATE($G$1,$H$1,A1,$I$2,$I$1,C1,$I$2,$J$1,$K$1)</f>
+        <v>{id: 3001, name: 'Apple Pie (Яблочный Пирог)', isSelected: false },</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -14651,8 +14651,8 @@
         <v>{name: 'Bilberry (Черника)' },</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M39" si="2">CONCATENATE($G$1,$H$1,A2,$I$2,$I$1,C2,$K$1)</f>
-        <v>{id: 3002, name: 'Bilberry (Черника)' },</v>
+        <f t="shared" ref="M2:M39" si="2">CONCATENATE($G$1,$H$1,A2,$I$2,$I$1,C2,$I$2,$J$1,$K$1)</f>
+        <v>{id: 3002, name: 'Bilberry (Черника)', isSelected: false },</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -14672,7 +14672,7 @@
       </c>
       <c r="M3" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3003, name: 'Biscotto Cookie (Овсяное Печенье)' },</v>
+        <v>{id: 3003, name: 'Biscotto Cookie (Овсяное Печенье)', isSelected: false },</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -14692,7 +14692,7 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3004, name: 'Blackberry (Ежевика)' },</v>
+        <v>{id: 3004, name: 'Blackberry (Ежевика)', isSelected: false },</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -14712,7 +14712,7 @@
       </c>
       <c r="M5" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3005, name: 'Blackcurrant (Черная Смородина)' },</v>
+        <v>{id: 3005, name: 'Blackcurrant (Черная Смородина)', isSelected: false },</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -14732,7 +14732,7 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3006, name: 'Caramel (Карамель)' },</v>
+        <v>{id: 3006, name: 'Caramel (Карамель)', isSelected: false },</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -14752,7 +14752,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3007, name: 'Champagne (Шампанское)' },</v>
+        <v>{id: 3007, name: 'Champagne (Шампанское)', isSelected: false },</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -14772,7 +14772,7 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3008, name: 'Cherry (Вишня)' },</v>
+        <v>{id: 3008, name: 'Cherry (Вишня)', isSelected: false },</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -14792,7 +14792,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3009, name: 'Citrus Mix (Цитрусовый Микс)' },</v>
+        <v>{id: 3009, name: 'Citrus Mix (Цитрусовый Микс)', isSelected: false },</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -14812,7 +14812,7 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3010, name: 'Classic Vanilla (Ваниль)' },</v>
+        <v>{id: 3010, name: 'Classic Vanilla (Ваниль)', isSelected: false },</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -14832,7 +14832,7 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3011, name: 'Coconut (Кокос)' },</v>
+        <v>{id: 3011, name: 'Coconut (Кокос)', isSelected: false },</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -14852,7 +14852,7 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3012, name: 'Cola (Кола)' },</v>
+        <v>{id: 3012, name: 'Cola (Кола)', isSelected: false },</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -14872,7 +14872,7 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3013, name: 'Custard Cream (Заварной Крем)' },</v>
+        <v>{id: 3013, name: 'Custard Cream (Заварной Крем)', isSelected: false },</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -14892,7 +14892,7 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3014, name: 'Forest Fruit Mix (Фруктовый Микс)' },</v>
+        <v>{id: 3014, name: 'Forest Fruit Mix (Фруктовый Микс)', isSelected: false },</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -14912,7 +14912,7 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3015, name: 'Fuji Apple (Яблоко Fuji)' },</v>
+        <v>{id: 3015, name: 'Fuji Apple (Яблоко Fuji)', isSelected: false },</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -14932,7 +14932,7 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3016, name: 'Green Tea (Зеленый Чай)' },</v>
+        <v>{id: 3016, name: 'Green Tea (Зеленый Чай)', isSelected: false },</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -14952,7 +14952,7 @@
       </c>
       <c r="M17" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3017, name: 'Hazelnut (Лесной Орех)' },</v>
+        <v>{id: 3017, name: 'Hazelnut (Лесной Орех)', isSelected: false },</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -14972,7 +14972,7 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3018, name: 'Kiwi (Киви)' },</v>
+        <v>{id: 3018, name: 'Kiwi (Киви)', isSelected: false },</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -14992,7 +14992,7 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3019, name: 'Lemon Sicily (Лимон Сицилийский)' },</v>
+        <v>{id: 3019, name: 'Lemon Sicily (Лимон Сицилийский)', isSelected: false },</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -15012,7 +15012,7 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3020, name: 'Lime Tahity Distilled (Лайм)' },</v>
+        <v>{id: 3020, name: 'Lime Tahity Distilled (Лайм)', isSelected: false },</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -15032,7 +15032,7 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3021, name: 'Mandarin (Мандарин)' },</v>
+        <v>{id: 3021, name: 'Mandarin (Мандарин)', isSelected: false },</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -15052,7 +15052,7 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3022, name: 'Mango (Манго)' },</v>
+        <v>{id: 3022, name: 'Mango (Манго)', isSelected: false },</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -15072,7 +15072,7 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3023, name: 'Marshmallow (Зефир)' },</v>
+        <v>{id: 3023, name: 'Marshmallow (Зефир)', isSelected: false },</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -15092,7 +15092,7 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3024, name: 'Maxx Blend (Табак Maxx Blend)' },</v>
+        <v>{id: 3024, name: 'Maxx Blend (Табак Maxx Blend)', isSelected: false },</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -15112,7 +15112,7 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3025, name: 'Melon Cantaloupe (Мускусная Дыня)' },</v>
+        <v>{id: 3025, name: 'Melon Cantaloupe (Мускусная Дыня)', isSelected: false },</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -15132,7 +15132,7 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3026, name: 'Menthol (Ментол)' },</v>
+        <v>{id: 3026, name: 'Menthol (Ментол)', isSelected: false },</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -15152,7 +15152,7 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3027, name: 'Meringue (Безе)' },</v>
+        <v>{id: 3027, name: 'Meringue (Безе)', isSelected: false },</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -15172,7 +15172,7 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3028, name: 'Nonna’s Cake (Пирог Нонны)' },</v>
+        <v>{id: 3028, name: 'Nonna’s Cake (Пирог Нонны)', isSelected: false },</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -15192,7 +15192,7 @@
       </c>
       <c r="M29" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3029, name: 'Orange (Апельсин)' },</v>
+        <v>{id: 3029, name: 'Orange (Апельсин)', isSelected: false },</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -15212,7 +15212,7 @@
       </c>
       <c r="M30" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3030, name: 'Passionfruit (Маракуйя)' },</v>
+        <v>{id: 3030, name: 'Passionfruit (Маракуйя)', isSelected: false },</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -15232,7 +15232,7 @@
       </c>
       <c r="M31" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3031, name: 'Raspberry (Малина)' },</v>
+        <v>{id: 3031, name: 'Raspberry (Малина)', isSelected: false },</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -15252,7 +15252,7 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3032, name: 'Soho (Табак Soho)' },</v>
+        <v>{id: 3032, name: 'Soho (Табак Soho)', isSelected: false },</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -15272,7 +15272,7 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3033, name: 'Spearmint (Мятная Жвачка)' },</v>
+        <v>{id: 3033, name: 'Spearmint (Мятная Жвачка)', isSelected: false },</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -15292,7 +15292,7 @@
       </c>
       <c r="M34" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3034, name: 'Stark Apple (Яблоко Красное)' },</v>
+        <v>{id: 3034, name: 'Stark Apple (Яблоко Красное)', isSelected: false },</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -15312,7 +15312,7 @@
       </c>
       <c r="M35" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3035, name: 'Strawberry (Клубника)' },</v>
+        <v>{id: 3035, name: 'Strawberry (Клубника)', isSelected: false },</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -15332,7 +15332,7 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3036, name: 'Virginia (Табак Virginia)' },</v>
+        <v>{id: 3036, name: 'Virginia (Табак Virginia)', isSelected: false },</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -15352,7 +15352,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3037, name: 'Watermelon (Арбуз)' },</v>
+        <v>{id: 3037, name: 'Watermelon (Арбуз)', isSelected: false },</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -15372,7 +15372,7 @@
       </c>
       <c r="M38" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3038, name: 'White Peach (Белый Персик)' },</v>
+        <v>{id: 3038, name: 'White Peach (Белый Персик)', isSelected: false },</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -15392,7 +15392,7 @@
       </c>
       <c r="M39" t="str">
         <f t="shared" si="2"/>
-        <v>{id: 3039, name: 'Yogurt (Йогурт)' },</v>
+        <v>{id: 3039, name: 'Yogurt (Йогурт)', isSelected: false },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>